<commit_message>
various corrections in progress tracking docs
</commit_message>
<xml_diff>
--- a/Progress Tracking/FFXI - Base - Mythic Weapon Progress.xlsx
+++ b/Progress Tracking/FFXI - Base - Mythic Weapon Progress.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Final Fantasy XI\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spanish\Dropbox\Windower4\addons\GearSwap\libs\Progress Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85401BD6-A08F-4219-A5B7-D37477C263C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63AFDB3-4C2F-417D-AAD8-49C4FA19B3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0B085B93-25BD-4630-92B3-1D4A9D01D8D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{0B085B93-25BD-4630-92B3-1D4A9D01D8D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
-    <sheet name="General" sheetId="3" r:id="rId2"/>
-    <sheet name="Assault Progress" sheetId="2" r:id="rId3"/>
-    <sheet name="Titles" sheetId="4" r:id="rId4"/>
-    <sheet name="Salvage Tracking" sheetId="5" r:id="rId5"/>
+    <sheet name="General" sheetId="3" r:id="rId1"/>
+    <sheet name="Assault Progress" sheetId="2" r:id="rId2"/>
+    <sheet name="Titles" sheetId="4" r:id="rId3"/>
+    <sheet name="Salvage Tracking" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="253">
   <si>
     <t>Leujaoam Sanctum</t>
   </si>
@@ -597,9 +596,6 @@
     <t>Long-Bowed Chariot (Bhaflau Remnants)</t>
   </si>
   <si>
-    <t>Got</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -793,6 +789,15 @@
   </si>
   <si>
     <t>Example</t>
+  </si>
+  <si>
+    <t>Acquired</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Title Progress</t>
   </si>
 </sst>
 </file>
@@ -1519,73 +1524,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1594,7 +1599,17 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1625,17 +1640,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{238A975E-00AE-4EBB-BB59-D6B13A141D44}" name="Table2" displayName="Table2" ref="B9:H27" totalsRowShown="0">
-  <autoFilter ref="B9:H27" xr:uid="{EDCDF189-9CAE-47D2-895A-26C70515F972}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{238A975E-00AE-4EBB-BB59-D6B13A141D44}" name="Table2" displayName="Table2" ref="B6:H24" totalsRowShown="0">
+  <autoFilter ref="B6:H24" xr:uid="{EDCDF189-9CAE-47D2-895A-26C70515F972}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{59BD3A02-2D89-4BE7-9508-4A372593E589}" name="Date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{59BD3A02-2D89-4BE7-9508-4A372593E589}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0A92B7D1-766D-4BB2-9B1D-0B241C7C599A}" name="Singles"/>
     <tableColumn id="3" xr3:uid="{07CF0ABD-5247-42B8-9314-1C7DE5DC1978}" name="Cotton Purses"/>
     <tableColumn id="4" xr3:uid="{280537A0-BCE8-4422-84AA-7B5F02CC32AA}" name="Cotton (Singles)"/>
     <tableColumn id="5" xr3:uid="{5A06AD49-3225-4A16-9C73-067A768DBE49}" name="Linen Purses"/>
     <tableColumn id="6" xr3:uid="{02D342FF-B933-47CD-AD84-077DBDF9C434}" name="Linen (Singles)"/>
     <tableColumn id="7" xr3:uid="{27484B81-EB68-40D0-8372-F3236E9E3B2C}" name="Total">
-      <calculatedColumnFormula>SUM(C10,E10,G10)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(C7,E7,G7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1643,10 +1658,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64D54E4A-1F87-4BD8-903B-33C9898C5A16}" name="Table24" displayName="Table24" ref="N9:T11" totalsRowShown="0">
-  <autoFilter ref="N9:T11" xr:uid="{AE317730-AC5C-497E-987F-785D2A1678B9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64D54E4A-1F87-4BD8-903B-33C9898C5A16}" name="Table24" displayName="Table24" ref="N6:T8" totalsRowShown="0">
+  <autoFilter ref="N6:T8" xr:uid="{AE317730-AC5C-497E-987F-785D2A1678B9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{42B95A70-C3D7-4095-9E1D-83CFF49EAF8B}" name="Date" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{42B95A70-C3D7-4095-9E1D-83CFF49EAF8B}" name="Date" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{125F5CC4-B418-4B38-BE3D-8B8D0FB458AA}" name="Singles"/>
     <tableColumn id="3" xr3:uid="{047A8502-115C-4B93-99A0-FC7320D3AAFF}" name="Cotton Purses"/>
     <tableColumn id="4" xr3:uid="{F490F338-FD4B-498A-8579-F32B01CB7339}" name="Cotton (Singles)"/>
@@ -1954,58 +1969,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AF42CF-8067-45EB-A782-722DE2E37D34}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5C447E-B1C7-48FC-86FA-81F2301FB971}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19"/>
       <c r="B1" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="30" t="s">
         <v>200</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>201</v>
       </c>
       <c r="E1" s="35"/>
       <c r="F1" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="43">
         <v>150000</v>
@@ -2022,10 +2025,10 @@
         <f>IF((C2/B2) &gt; 1, 1, C2/B2)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="85" t="s">
-        <v>224</v>
-      </c>
-      <c r="I2" s="86"/>
+      <c r="H2" s="97" t="s">
+        <v>223</v>
+      </c>
+      <c r="I2" s="98"/>
       <c r="J2" s="28">
         <v>960</v>
       </c>
@@ -2034,9 +2037,9 @@
         <v>960</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="20">
         <v>100000</v>
@@ -2053,10 +2056,10 @@
         <f>IF((C3/B3) &gt; 1, 1, C3/B3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="78" t="s">
-        <v>223</v>
-      </c>
-      <c r="I3" s="79"/>
+      <c r="H3" s="90" t="s">
+        <v>222</v>
+      </c>
+      <c r="I3" s="91"/>
       <c r="J3" s="53">
         <v>1440</v>
       </c>
@@ -2065,9 +2068,9 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" s="20">
         <v>30000</v>
@@ -2084,10 +2087,10 @@
         <f>IF((C4/B4) &gt; 1, 1, C4/B4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="78" t="s">
-        <v>203</v>
-      </c>
-      <c r="I4" s="79"/>
+      <c r="H4" s="90" t="s">
+        <v>202</v>
+      </c>
+      <c r="I4" s="91"/>
       <c r="J4" s="54">
         <v>1920</v>
       </c>
@@ -2096,9 +2099,9 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B5" s="22">
         <v>10000</v>
@@ -2115,20 +2118,20 @@
         <f>IF((H19/B5) &gt; 1, 1, H19/B5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="80" t="s">
-        <v>204</v>
-      </c>
-      <c r="I5" s="81"/>
+      <c r="H5" s="92" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="93"/>
       <c r="J5" s="71">
         <f>ROUNDUP((D3/J4),0)</f>
         <v>53</v>
       </c>
       <c r="K5" s="74"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>6</v>
@@ -2155,16 +2158,16 @@
         <v>34</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K8" s="30" t="s">
         <v>42</v>
       </c>
       <c r="L8" s="70" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>0</v>
       </c>
@@ -2213,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>46</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>79</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>110</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
         <v>136</v>
       </c>
@@ -2409,34 +2412,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L14" s="70">
         <f>(SUM(L9:L13)/5)</f>
         <v>0</v>
       </c>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F15" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="H15" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="H15" s="51" t="s">
-        <v>220</v>
-      </c>
       <c r="I15" s="57"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="28">
@@ -2452,16 +2455,16 @@
       </c>
       <c r="I16" s="58"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B17" s="40">
         <f>F4</f>
         <v>0</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="29">
@@ -2477,40 +2480,40 @@
       </c>
       <c r="I17" s="58"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" s="40">
         <f>L14</f>
         <v>0</v>
       </c>
-      <c r="D18" s="82" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
+      <c r="D18" s="94" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="96"/>
       <c r="H18" s="51">
         <f>SUM(H16:H17)</f>
         <v>0</v>
       </c>
       <c r="I18" s="56"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19" s="40">
         <f>F3</f>
         <v>0</v>
       </c>
-      <c r="D19" s="82" t="s">
-        <v>222</v>
-      </c>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="84"/>
+      <c r="D19" s="94" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="96"/>
       <c r="H19" s="52">
         <f>H18+C5</f>
         <v>0</v>
@@ -2520,43 +2523,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20" s="40">
         <f>F2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="B21" s="40">
+        <f>COUNTIF(Titles!C2:C9,"Yes")/COUNTA(Titles!A2:A9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="B22" s="40">
         <f>I19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="62"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>215</v>
-      </c>
-      <c r="B23" s="40">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="38"/>
+      <c r="B23" s="62"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" s="40">
         <f>AVERAGE(B17:B20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="B24" s="47">
-        <f>AVERAGE(B17:B21)</f>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="47">
+        <f>AVERAGE(B17:B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -2569,11 +2581,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B17:B24 F2:F6 L9:L14">
+  <conditionalFormatting sqref="B17:B25 F2:F6 L9:L14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
@@ -2587,167 +2599,167 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA460102-6C51-4136-B769-64E054CD3D0F}">
   <dimension ref="A1:AM19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="4"/>
-    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="3"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="3"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" style="3"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.85546875" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" customWidth="1"/>
-    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.85546875" customWidth="1"/>
-    <col min="33" max="33" width="8.85546875" style="3"/>
-    <col min="34" max="34" width="14.42578125" customWidth="1"/>
-    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.85546875" customWidth="1"/>
-    <col min="37" max="38" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.140625" style="14"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="3"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="3"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" customWidth="1"/>
+    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.88671875" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" style="3"/>
+    <col min="26" max="26" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.88671875" customWidth="1"/>
+    <col min="28" max="28" width="19.44140625" customWidth="1"/>
+    <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" customWidth="1"/>
+    <col min="33" max="33" width="8.88671875" style="3"/>
+    <col min="34" max="34" width="14.44140625" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.88671875" customWidth="1"/>
+    <col min="37" max="38" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="G1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="I1" s="92" t="s">
+    <row r="1" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="G1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="O1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q1" s="92" t="s">
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="O1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q1" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="W1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="Y1" s="92" t="s">
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="W1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y1" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93"/>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="AE1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="AG1" s="92" t="s">
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="AE1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="AG1" s="104" t="s">
         <v>136</v>
       </c>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93"/>
-      <c r="AJ1" s="93"/>
-      <c r="AK1" s="93"/>
-      <c r="AL1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="AM1" s="89" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87" t="s">
+      <c r="AH1" s="105"/>
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="105"/>
+      <c r="AK1" s="105"/>
+      <c r="AL1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="AM1" s="101" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="I2" s="92" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="I2" s="104" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="Q2" s="92" t="s">
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="Q2" s="104" t="s">
         <v>169</v>
       </c>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="Y2" s="92" t="s">
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="Y2" s="104" t="s">
         <v>170</v>
       </c>
-      <c r="Z2" s="93"/>
-      <c r="AA2" s="93"/>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="93"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="90"/>
-      <c r="AG2" s="92" t="s">
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="102"/>
+      <c r="AG2" s="104" t="s">
         <v>171</v>
       </c>
-      <c r="AH2" s="93"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="93"/>
-      <c r="AK2" s="93"/>
-      <c r="AL2" s="90"/>
-      <c r="AM2" s="90"/>
-    </row>
-    <row r="3" spans="1:39" s="5" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="102"/>
+      <c r="AM2" s="102"/>
+    </row>
+    <row r="3" spans="1:39" s="5" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2763,8 +2775,8 @@
       <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
       <c r="I3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2780,8 +2792,8 @@
       <c r="M3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
       <c r="Q3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2797,8 +2809,8 @@
       <c r="U3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="103"/>
       <c r="Y3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2814,8 +2826,8 @@
       <c r="AC3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="91"/>
+      <c r="AD3" s="103"/>
+      <c r="AE3" s="103"/>
       <c r="AG3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2831,10 +2843,10 @@
       <c r="AK3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AL3" s="91"/>
-      <c r="AM3" s="91"/>
-    </row>
-    <row r="4" spans="1:39" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="AL3" s="103"/>
+      <c r="AM3" s="103"/>
+    </row>
+    <row r="4" spans="1:39" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -2850,7 +2862,9 @@
       <c r="E4" s="14">
         <v>1000</v>
       </c>
-      <c r="F4" s="77"/>
+      <c r="F4" s="77" t="s">
+        <v>251</v>
+      </c>
       <c r="G4" s="63"/>
       <c r="I4" s="9" t="s">
         <v>6</v>
@@ -2921,7 +2935,7 @@
       <c r="AL4" s="77"/>
       <c r="AM4" s="77"/>
     </row>
-    <row r="5" spans="1:39" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -3003,12 +3017,12 @@
         <v>142</v>
       </c>
       <c r="AK5" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL5" s="63"/>
       <c r="AM5" s="63"/>
     </row>
-    <row r="6" spans="1:39" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
@@ -3090,12 +3104,12 @@
         <v>145</v>
       </c>
       <c r="AK6" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AL6" s="63"/>
       <c r="AM6" s="63"/>
     </row>
-    <row r="7" spans="1:39" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
@@ -3177,12 +3191,12 @@
         <v>148</v>
       </c>
       <c r="AK7" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL7" s="63"/>
       <c r="AM7" s="68"/>
     </row>
-    <row r="8" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="102" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
@@ -3269,7 +3283,7 @@
       <c r="AL8" s="63"/>
       <c r="AM8" s="63"/>
     </row>
-    <row r="9" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
@@ -3300,7 +3314,7 @@
         <v>64</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N9" s="63"/>
       <c r="O9" s="63"/>
@@ -3356,7 +3370,7 @@
       <c r="AL9" s="63"/>
       <c r="AM9" s="63"/>
     </row>
-    <row r="10" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
@@ -3443,7 +3457,7 @@
       <c r="AL10" s="63"/>
       <c r="AM10" s="63"/>
     </row>
-    <row r="11" spans="1:39" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" ht="122.4" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -3530,7 +3544,7 @@
       <c r="AL11" s="63"/>
       <c r="AM11" s="63"/>
     </row>
-    <row r="12" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" ht="102" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>38</v>
       </c>
@@ -3617,7 +3631,7 @@
       <c r="AL12" s="63"/>
       <c r="AM12" s="63"/>
     </row>
-    <row r="13" spans="1:39" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="112.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
@@ -3704,16 +3718,16 @@
       <c r="AL13" s="64"/>
       <c r="AM13" s="64"/>
     </row>
-    <row r="14" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" s="2"/>
     </row>
   </sheetData>
@@ -3740,7 +3754,7 @@
     <mergeCell ref="I1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 N1:O1 V1:W1 AD1:AE1 AL1:AM1 AG1:AG2 G2:G3 O2:O3 W2:W3 AE2:AE3 AM2:AM3 AG3:AK3 F4:G1048576 N4:O1048576 V4:W1048576 AD4:AE1048576 AG4:AM1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3749,408 +3763,414 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B18E4BA-209E-45D4-84F2-5131F8B6487E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="80" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="85"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="87" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="98" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="99" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="101" t="s">
+      <c r="C3" s="88"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="84" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="102"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="104" t="s">
-        <v>188</v>
-      </c>
-      <c r="C3" s="105"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
-        <v>180</v>
-      </c>
-      <c r="B4" s="101" t="s">
+      <c r="C4" s="85"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="86" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="88"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="83" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="85"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="88"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="83" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="85"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="78" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="102"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="104" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="105"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="101" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" s="102"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" s="104" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="105"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="100" t="s">
-        <v>183</v>
-      </c>
-      <c r="B8" s="101" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="102"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="95" t="s">
-        <v>184</v>
-      </c>
-      <c r="B9" s="96" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="106"/>
+      <c r="C9" s="89"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708861EB-D3EE-4006-B4B0-E960B9A7079E}">
-  <dimension ref="A5:W27"/>
+  <dimension ref="A2:W24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="94" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="59" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="B4" s="106" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="N4" s="106" t="s">
         <v>238</v>
       </c>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="N7" s="94" t="s">
-        <v>239</v>
-      </c>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="94"/>
-      <c r="V7" t="s">
-        <v>237</v>
-      </c>
-      <c r="W7">
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="106"/>
+      <c r="S4" s="106"/>
+      <c r="T4" s="106"/>
+      <c r="V4" t="s">
+        <v>236</v>
+      </c>
+      <c r="W4">
         <f>COUNTA(N:N)-2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="59" t="s">
+    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" t="s">
         <v>226</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H6" t="s">
         <v>227</v>
       </c>
-      <c r="D9" t="s">
-        <v>231</v>
-      </c>
-      <c r="E9" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" t="s">
-        <v>232</v>
-      </c>
-      <c r="H9" t="s">
-        <v>228</v>
-      </c>
-      <c r="J9" s="75" t="s">
-        <v>237</v>
-      </c>
-      <c r="K9" s="76">
+      <c r="J6" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="K6" s="76">
         <f>COUNTA(B:B)-2</f>
         <v>1</v>
       </c>
-      <c r="N9" s="59" t="s">
+      <c r="N6" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="O6" t="s">
         <v>226</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>229</v>
+      </c>
+      <c r="R6" t="s">
+        <v>228</v>
+      </c>
+      <c r="S6" t="s">
+        <v>231</v>
+      </c>
+      <c r="T6" t="s">
         <v>227</v>
       </c>
-      <c r="P9" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>230</v>
-      </c>
-      <c r="R9" t="s">
-        <v>229</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="V6" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="W6" s="41">
+        <f>AVERAGE(O:O)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="59">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="59">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="V7" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="T9" t="s">
-        <v>228</v>
-      </c>
-      <c r="V9" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="W9" s="41">
-        <f>AVERAGE(O:O)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="59">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="V10" s="37" t="s">
+      <c r="W7" s="60">
+        <f>AVERAGE(Q:Q)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B8" s="59"/>
+      <c r="J8" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="K8" s="41">
+        <f>ROUNDDOWN(AVERAGE(C:C), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="59"/>
+      <c r="V8" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="W10" s="60">
-        <f>AVERAGE(Q:Q)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="59"/>
-      <c r="J11" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="K11" s="41">
-        <f>ROUNDDOWN(AVERAGE(C:C), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="59"/>
-      <c r="V11" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="W11" s="60">
+      <c r="W8" s="60">
         <f>AVERAGE(S:S)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="59"/>
-      <c r="J12" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="K12" s="60" t="e">
+    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="59"/>
+      <c r="J9" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="K9" s="60" t="e">
         <f>ROUNDDOWN(SUM(E:E)/COUNTIF(E:E,"&gt;0"), 0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V12" s="49" t="s">
-        <v>236</v>
-      </c>
-      <c r="W12" s="61">
+      <c r="V9" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="W9" s="61">
         <f>AVERAGE(T:T)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="59"/>
-      <c r="J13" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="K13" s="60" t="e">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B10" s="59"/>
+      <c r="J10" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="K10" s="60" t="e">
         <f>ROUNDDOWN(SUM(G:G)/COUNTIF(G:G,"&gt;0"), 0)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="59"/>
+      <c r="J11" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="K11" s="61">
+        <f>ROUNDDOWN(AVERAGE(H:H), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="59"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B13" s="59"/>
+      <c r="J13" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="K13" s="41">
+        <f>SUM(C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B14" s="59"/>
-      <c r="J14" s="49" t="s">
-        <v>236</v>
-      </c>
-      <c r="K14" s="61">
-        <f>ROUNDDOWN(AVERAGE(H:H), 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14" s="60">
+        <f>SUM(E:E)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="59"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J15" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="K15" s="61">
+        <f>SUM(G:G)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="59"/>
-      <c r="J16" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="K16" s="41">
-        <f>SUM(C:C)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="K16" s="61">
+        <f>SUM(K13:K15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="59"/>
-      <c r="J17" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="K17" s="60">
-        <f>SUM(E:E)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="59"/>
-      <c r="J18" s="49" t="s">
-        <v>246</v>
-      </c>
-      <c r="K18" s="61">
-        <f>SUM(G:G)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="59"/>
-      <c r="J19" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="K19" s="61">
-        <f>SUM(K16:K18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="59"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="59"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="59"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="59"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="59"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="2">
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="N4:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Misc October-2024 Updates & Upkeep (#33)
* various corrections in progress tracking docs

* cor gear updates

* drg gear updates

* whm gear updates

* whm main lua updates

* sch gear updates

* sch main lua updates
</commit_message>
<xml_diff>
--- a/Progress Tracking/FFXI - Base - Mythic Weapon Progress.xlsx
+++ b/Progress Tracking/FFXI - Base - Mythic Weapon Progress.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Final Fantasy XI\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spanish\Dropbox\Windower4\addons\GearSwap\libs\Progress Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85401BD6-A08F-4219-A5B7-D37477C263C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63AFDB3-4C2F-417D-AAD8-49C4FA19B3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0B085B93-25BD-4630-92B3-1D4A9D01D8D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{0B085B93-25BD-4630-92B3-1D4A9D01D8D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
-    <sheet name="General" sheetId="3" r:id="rId2"/>
-    <sheet name="Assault Progress" sheetId="2" r:id="rId3"/>
-    <sheet name="Titles" sheetId="4" r:id="rId4"/>
-    <sheet name="Salvage Tracking" sheetId="5" r:id="rId5"/>
+    <sheet name="General" sheetId="3" r:id="rId1"/>
+    <sheet name="Assault Progress" sheetId="2" r:id="rId2"/>
+    <sheet name="Titles" sheetId="4" r:id="rId3"/>
+    <sheet name="Salvage Tracking" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="253">
   <si>
     <t>Leujaoam Sanctum</t>
   </si>
@@ -597,9 +596,6 @@
     <t>Long-Bowed Chariot (Bhaflau Remnants)</t>
   </si>
   <si>
-    <t>Got</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -793,6 +789,15 @@
   </si>
   <si>
     <t>Example</t>
+  </si>
+  <si>
+    <t>Acquired</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Title Progress</t>
   </si>
 </sst>
 </file>
@@ -1519,73 +1524,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1594,7 +1599,17 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1625,17 +1640,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{238A975E-00AE-4EBB-BB59-D6B13A141D44}" name="Table2" displayName="Table2" ref="B9:H27" totalsRowShown="0">
-  <autoFilter ref="B9:H27" xr:uid="{EDCDF189-9CAE-47D2-895A-26C70515F972}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{238A975E-00AE-4EBB-BB59-D6B13A141D44}" name="Table2" displayName="Table2" ref="B6:H24" totalsRowShown="0">
+  <autoFilter ref="B6:H24" xr:uid="{EDCDF189-9CAE-47D2-895A-26C70515F972}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{59BD3A02-2D89-4BE7-9508-4A372593E589}" name="Date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{59BD3A02-2D89-4BE7-9508-4A372593E589}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0A92B7D1-766D-4BB2-9B1D-0B241C7C599A}" name="Singles"/>
     <tableColumn id="3" xr3:uid="{07CF0ABD-5247-42B8-9314-1C7DE5DC1978}" name="Cotton Purses"/>
     <tableColumn id="4" xr3:uid="{280537A0-BCE8-4422-84AA-7B5F02CC32AA}" name="Cotton (Singles)"/>
     <tableColumn id="5" xr3:uid="{5A06AD49-3225-4A16-9C73-067A768DBE49}" name="Linen Purses"/>
     <tableColumn id="6" xr3:uid="{02D342FF-B933-47CD-AD84-077DBDF9C434}" name="Linen (Singles)"/>
     <tableColumn id="7" xr3:uid="{27484B81-EB68-40D0-8372-F3236E9E3B2C}" name="Total">
-      <calculatedColumnFormula>SUM(C10,E10,G10)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(C7,E7,G7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1643,10 +1658,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64D54E4A-1F87-4BD8-903B-33C9898C5A16}" name="Table24" displayName="Table24" ref="N9:T11" totalsRowShown="0">
-  <autoFilter ref="N9:T11" xr:uid="{AE317730-AC5C-497E-987F-785D2A1678B9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64D54E4A-1F87-4BD8-903B-33C9898C5A16}" name="Table24" displayName="Table24" ref="N6:T8" totalsRowShown="0">
+  <autoFilter ref="N6:T8" xr:uid="{AE317730-AC5C-497E-987F-785D2A1678B9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{42B95A70-C3D7-4095-9E1D-83CFF49EAF8B}" name="Date" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{42B95A70-C3D7-4095-9E1D-83CFF49EAF8B}" name="Date" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{125F5CC4-B418-4B38-BE3D-8B8D0FB458AA}" name="Singles"/>
     <tableColumn id="3" xr3:uid="{047A8502-115C-4B93-99A0-FC7320D3AAFF}" name="Cotton Purses"/>
     <tableColumn id="4" xr3:uid="{F490F338-FD4B-498A-8579-F32B01CB7339}" name="Cotton (Singles)"/>
@@ -1954,58 +1969,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AF42CF-8067-45EB-A782-722DE2E37D34}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5C447E-B1C7-48FC-86FA-81F2301FB971}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19"/>
       <c r="B1" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="30" t="s">
         <v>200</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>201</v>
       </c>
       <c r="E1" s="35"/>
       <c r="F1" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="43">
         <v>150000</v>
@@ -2022,10 +2025,10 @@
         <f>IF((C2/B2) &gt; 1, 1, C2/B2)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="85" t="s">
-        <v>224</v>
-      </c>
-      <c r="I2" s="86"/>
+      <c r="H2" s="97" t="s">
+        <v>223</v>
+      </c>
+      <c r="I2" s="98"/>
       <c r="J2" s="28">
         <v>960</v>
       </c>
@@ -2034,9 +2037,9 @@
         <v>960</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="20">
         <v>100000</v>
@@ -2053,10 +2056,10 @@
         <f>IF((C3/B3) &gt; 1, 1, C3/B3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="78" t="s">
-        <v>223</v>
-      </c>
-      <c r="I3" s="79"/>
+      <c r="H3" s="90" t="s">
+        <v>222</v>
+      </c>
+      <c r="I3" s="91"/>
       <c r="J3" s="53">
         <v>1440</v>
       </c>
@@ -2065,9 +2068,9 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" s="20">
         <v>30000</v>
@@ -2084,10 +2087,10 @@
         <f>IF((C4/B4) &gt; 1, 1, C4/B4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="78" t="s">
-        <v>203</v>
-      </c>
-      <c r="I4" s="79"/>
+      <c r="H4" s="90" t="s">
+        <v>202</v>
+      </c>
+      <c r="I4" s="91"/>
       <c r="J4" s="54">
         <v>1920</v>
       </c>
@@ -2096,9 +2099,9 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B5" s="22">
         <v>10000</v>
@@ -2115,20 +2118,20 @@
         <f>IF((H19/B5) &gt; 1, 1, H19/B5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="80" t="s">
-        <v>204</v>
-      </c>
-      <c r="I5" s="81"/>
+      <c r="H5" s="92" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="93"/>
       <c r="J5" s="71">
         <f>ROUNDUP((D3/J4),0)</f>
         <v>53</v>
       </c>
       <c r="K5" s="74"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>6</v>
@@ -2155,16 +2158,16 @@
         <v>34</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K8" s="30" t="s">
         <v>42</v>
       </c>
       <c r="L8" s="70" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>0</v>
       </c>
@@ -2213,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>46</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>79</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>110</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
         <v>136</v>
       </c>
@@ -2409,34 +2412,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L14" s="70">
         <f>(SUM(L9:L13)/5)</f>
         <v>0</v>
       </c>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F15" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="H15" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="H15" s="51" t="s">
-        <v>220</v>
-      </c>
       <c r="I15" s="57"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="28">
@@ -2452,16 +2455,16 @@
       </c>
       <c r="I16" s="58"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B17" s="40">
         <f>F4</f>
         <v>0</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="29">
@@ -2477,40 +2480,40 @@
       </c>
       <c r="I17" s="58"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" s="40">
         <f>L14</f>
         <v>0</v>
       </c>
-      <c r="D18" s="82" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
+      <c r="D18" s="94" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="96"/>
       <c r="H18" s="51">
         <f>SUM(H16:H17)</f>
         <v>0</v>
       </c>
       <c r="I18" s="56"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19" s="40">
         <f>F3</f>
         <v>0</v>
       </c>
-      <c r="D19" s="82" t="s">
-        <v>222</v>
-      </c>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="84"/>
+      <c r="D19" s="94" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="96"/>
       <c r="H19" s="52">
         <f>H18+C5</f>
         <v>0</v>
@@ -2520,43 +2523,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20" s="40">
         <f>F2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="B21" s="40">
+        <f>COUNTIF(Titles!C2:C9,"Yes")/COUNTA(Titles!A2:A9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="B22" s="40">
         <f>I19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="62"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>215</v>
-      </c>
-      <c r="B23" s="40">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="38"/>
+      <c r="B23" s="62"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" s="40">
         <f>AVERAGE(B17:B20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="B24" s="47">
-        <f>AVERAGE(B17:B21)</f>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="47">
+        <f>AVERAGE(B17:B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -2569,11 +2581,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B17:B24 F2:F6 L9:L14">
+  <conditionalFormatting sqref="B17:B25 F2:F6 L9:L14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
@@ -2587,167 +2599,167 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA460102-6C51-4136-B769-64E054CD3D0F}">
   <dimension ref="A1:AM19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="4"/>
-    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="3"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="3"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" style="3"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.85546875" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" customWidth="1"/>
-    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.85546875" customWidth="1"/>
-    <col min="33" max="33" width="8.85546875" style="3"/>
-    <col min="34" max="34" width="14.42578125" customWidth="1"/>
-    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.85546875" customWidth="1"/>
-    <col min="37" max="38" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.140625" style="14"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="3"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="3"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" customWidth="1"/>
+    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.88671875" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" style="3"/>
+    <col min="26" max="26" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.88671875" customWidth="1"/>
+    <col min="28" max="28" width="19.44140625" customWidth="1"/>
+    <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" customWidth="1"/>
+    <col min="33" max="33" width="8.88671875" style="3"/>
+    <col min="34" max="34" width="14.44140625" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.88671875" customWidth="1"/>
+    <col min="37" max="38" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="G1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="I1" s="92" t="s">
+    <row r="1" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="G1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="O1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q1" s="92" t="s">
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="O1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q1" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="W1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="Y1" s="92" t="s">
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="W1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y1" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93"/>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="AE1" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="AG1" s="92" t="s">
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="AE1" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="AG1" s="104" t="s">
         <v>136</v>
       </c>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93"/>
-      <c r="AJ1" s="93"/>
-      <c r="AK1" s="93"/>
-      <c r="AL1" s="89" t="s">
-        <v>249</v>
-      </c>
-      <c r="AM1" s="89" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87" t="s">
+      <c r="AH1" s="105"/>
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="105"/>
+      <c r="AK1" s="105"/>
+      <c r="AL1" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="AM1" s="101" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="I2" s="92" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="I2" s="104" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="Q2" s="92" t="s">
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="Q2" s="104" t="s">
         <v>169</v>
       </c>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="Y2" s="92" t="s">
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="Y2" s="104" t="s">
         <v>170</v>
       </c>
-      <c r="Z2" s="93"/>
-      <c r="AA2" s="93"/>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="93"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="90"/>
-      <c r="AG2" s="92" t="s">
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="102"/>
+      <c r="AG2" s="104" t="s">
         <v>171</v>
       </c>
-      <c r="AH2" s="93"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="93"/>
-      <c r="AK2" s="93"/>
-      <c r="AL2" s="90"/>
-      <c r="AM2" s="90"/>
-    </row>
-    <row r="3" spans="1:39" s="5" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="102"/>
+      <c r="AM2" s="102"/>
+    </row>
+    <row r="3" spans="1:39" s="5" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2763,8 +2775,8 @@
       <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
       <c r="I3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2780,8 +2792,8 @@
       <c r="M3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
       <c r="Q3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2797,8 +2809,8 @@
       <c r="U3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="103"/>
       <c r="Y3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2814,8 +2826,8 @@
       <c r="AC3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="91"/>
+      <c r="AD3" s="103"/>
+      <c r="AE3" s="103"/>
       <c r="AG3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2831,10 +2843,10 @@
       <c r="AK3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AL3" s="91"/>
-      <c r="AM3" s="91"/>
-    </row>
-    <row r="4" spans="1:39" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="AL3" s="103"/>
+      <c r="AM3" s="103"/>
+    </row>
+    <row r="4" spans="1:39" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -2850,7 +2862,9 @@
       <c r="E4" s="14">
         <v>1000</v>
       </c>
-      <c r="F4" s="77"/>
+      <c r="F4" s="77" t="s">
+        <v>251</v>
+      </c>
       <c r="G4" s="63"/>
       <c r="I4" s="9" t="s">
         <v>6</v>
@@ -2921,7 +2935,7 @@
       <c r="AL4" s="77"/>
       <c r="AM4" s="77"/>
     </row>
-    <row r="5" spans="1:39" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -3003,12 +3017,12 @@
         <v>142</v>
       </c>
       <c r="AK5" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL5" s="63"/>
       <c r="AM5" s="63"/>
     </row>
-    <row r="6" spans="1:39" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
@@ -3090,12 +3104,12 @@
         <v>145</v>
       </c>
       <c r="AK6" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AL6" s="63"/>
       <c r="AM6" s="63"/>
     </row>
-    <row r="7" spans="1:39" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
@@ -3177,12 +3191,12 @@
         <v>148</v>
       </c>
       <c r="AK7" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL7" s="63"/>
       <c r="AM7" s="68"/>
     </row>
-    <row r="8" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="102" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
@@ -3269,7 +3283,7 @@
       <c r="AL8" s="63"/>
       <c r="AM8" s="63"/>
     </row>
-    <row r="9" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
@@ -3300,7 +3314,7 @@
         <v>64</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N9" s="63"/>
       <c r="O9" s="63"/>
@@ -3356,7 +3370,7 @@
       <c r="AL9" s="63"/>
       <c r="AM9" s="63"/>
     </row>
-    <row r="10" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
@@ -3443,7 +3457,7 @@
       <c r="AL10" s="63"/>
       <c r="AM10" s="63"/>
     </row>
-    <row r="11" spans="1:39" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" ht="122.4" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -3530,7 +3544,7 @@
       <c r="AL11" s="63"/>
       <c r="AM11" s="63"/>
     </row>
-    <row r="12" spans="1:39" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" ht="102" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>38</v>
       </c>
@@ -3617,7 +3631,7 @@
       <c r="AL12" s="63"/>
       <c r="AM12" s="63"/>
     </row>
-    <row r="13" spans="1:39" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="112.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
@@ -3704,16 +3718,16 @@
       <c r="AL13" s="64"/>
       <c r="AM13" s="64"/>
     </row>
-    <row r="14" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" s="2"/>
     </row>
   </sheetData>
@@ -3740,7 +3754,7 @@
     <mergeCell ref="I1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 N1:O1 V1:W1 AD1:AE1 AL1:AM1 AG1:AG2 G2:G3 O2:O3 W2:W3 AE2:AE3 AM2:AM3 AG3:AK3 F4:G1048576 N4:O1048576 V4:W1048576 AD4:AE1048576 AG4:AM1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3749,408 +3763,414 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B18E4BA-209E-45D4-84F2-5131F8B6487E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="80" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="85"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="87" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="98" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="99" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="101" t="s">
+      <c r="C3" s="88"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="84" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="102"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="104" t="s">
-        <v>188</v>
-      </c>
-      <c r="C3" s="105"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
-        <v>180</v>
-      </c>
-      <c r="B4" s="101" t="s">
+      <c r="C4" s="85"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="86" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="88"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="83" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="85"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="88"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="83" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="85"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="78" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="102"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="104" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="105"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="101" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" s="102"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" s="104" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="105"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="100" t="s">
-        <v>183</v>
-      </c>
-      <c r="B8" s="101" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="102"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="95" t="s">
-        <v>184</v>
-      </c>
-      <c r="B9" s="96" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="106"/>
+      <c r="C9" s="89"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708861EB-D3EE-4006-B4B0-E960B9A7079E}">
-  <dimension ref="A5:W27"/>
+  <dimension ref="A2:W24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="94" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="59" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="B4" s="106" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="N4" s="106" t="s">
         <v>238</v>
       </c>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="N7" s="94" t="s">
-        <v>239</v>
-      </c>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="94"/>
-      <c r="V7" t="s">
-        <v>237</v>
-      </c>
-      <c r="W7">
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="106"/>
+      <c r="S4" s="106"/>
+      <c r="T4" s="106"/>
+      <c r="V4" t="s">
+        <v>236</v>
+      </c>
+      <c r="W4">
         <f>COUNTA(N:N)-2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="59" t="s">
+    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" t="s">
         <v>226</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H6" t="s">
         <v>227</v>
       </c>
-      <c r="D9" t="s">
-        <v>231</v>
-      </c>
-      <c r="E9" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" t="s">
-        <v>232</v>
-      </c>
-      <c r="H9" t="s">
-        <v>228</v>
-      </c>
-      <c r="J9" s="75" t="s">
-        <v>237</v>
-      </c>
-      <c r="K9" s="76">
+      <c r="J6" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="K6" s="76">
         <f>COUNTA(B:B)-2</f>
         <v>1</v>
       </c>
-      <c r="N9" s="59" t="s">
+      <c r="N6" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="O6" t="s">
         <v>226</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>229</v>
+      </c>
+      <c r="R6" t="s">
+        <v>228</v>
+      </c>
+      <c r="S6" t="s">
+        <v>231</v>
+      </c>
+      <c r="T6" t="s">
         <v>227</v>
       </c>
-      <c r="P9" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>230</v>
-      </c>
-      <c r="R9" t="s">
-        <v>229</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="V6" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="W6" s="41">
+        <f>AVERAGE(O:O)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="59">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="59">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="V7" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="T9" t="s">
-        <v>228</v>
-      </c>
-      <c r="V9" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="W9" s="41">
-        <f>AVERAGE(O:O)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="59">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="V10" s="37" t="s">
+      <c r="W7" s="60">
+        <f>AVERAGE(Q:Q)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B8" s="59"/>
+      <c r="J8" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="K8" s="41">
+        <f>ROUNDDOWN(AVERAGE(C:C), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="59"/>
+      <c r="V8" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="W10" s="60">
-        <f>AVERAGE(Q:Q)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="59"/>
-      <c r="J11" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="K11" s="41">
-        <f>ROUNDDOWN(AVERAGE(C:C), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="59"/>
-      <c r="V11" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="W11" s="60">
+      <c r="W8" s="60">
         <f>AVERAGE(S:S)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="59"/>
-      <c r="J12" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="K12" s="60" t="e">
+    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="59"/>
+      <c r="J9" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="K9" s="60" t="e">
         <f>ROUNDDOWN(SUM(E:E)/COUNTIF(E:E,"&gt;0"), 0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V12" s="49" t="s">
-        <v>236</v>
-      </c>
-      <c r="W12" s="61">
+      <c r="V9" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="W9" s="61">
         <f>AVERAGE(T:T)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="59"/>
-      <c r="J13" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="K13" s="60" t="e">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B10" s="59"/>
+      <c r="J10" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="K10" s="60" t="e">
         <f>ROUNDDOWN(SUM(G:G)/COUNTIF(G:G,"&gt;0"), 0)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="59"/>
+      <c r="J11" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="K11" s="61">
+        <f>ROUNDDOWN(AVERAGE(H:H), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="59"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B13" s="59"/>
+      <c r="J13" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="K13" s="41">
+        <f>SUM(C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B14" s="59"/>
-      <c r="J14" s="49" t="s">
-        <v>236</v>
-      </c>
-      <c r="K14" s="61">
-        <f>ROUNDDOWN(AVERAGE(H:H), 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14" s="60">
+        <f>SUM(E:E)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="59"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J15" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="K15" s="61">
+        <f>SUM(G:G)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="59"/>
-      <c r="J16" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="K16" s="41">
-        <f>SUM(C:C)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="K16" s="61">
+        <f>SUM(K13:K15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="59"/>
-      <c r="J17" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="K17" s="60">
-        <f>SUM(E:E)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="59"/>
-      <c r="J18" s="49" t="s">
-        <v>246</v>
-      </c>
-      <c r="K18" s="61">
-        <f>SUM(G:G)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="59"/>
-      <c r="J19" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="K19" s="61">
-        <f>SUM(K16:K18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="59"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="59"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="59"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="59"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="59"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="2">
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="N4:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>